<commit_message>
chore: Update center_locations.json with additional items and fix get_center_locations_for_item function
</commit_message>
<xml_diff>
--- a/sim/products.xlsx
+++ b/sim/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yossi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/sd card/study/year_3/Picking/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B8C59B-C52F-4D21-A544-C92502F30CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3F7620-953F-4742-AF12-C600D5152C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B8B0D30-750C-4C9D-85A7-B34DFC43DEF5}"/>
+    <workbookView xWindow="4720" yWindow="0" windowWidth="23260" windowHeight="14020" xr2:uid="{6B8B0D30-750C-4C9D-85A7-B34DFC43DEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Familys" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Familys!$A$1:$C$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Familys!$A$1:$C$296</definedName>
     <definedName name="BlackFormats" localSheetId="0">#REF!</definedName>
     <definedName name="BlackFormats">#REF!</definedName>
     <definedName name="QTY">[1]Stikers!$S$6:$S$15,[1]Stikers!$AM$6:$AM$15,[1]Stikers!$S$22:$S$31,[1]Stikers!$AM$22:$AM$31</definedName>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
   <si>
     <t>item_id</t>
   </si>
@@ -935,6 +935,21 @@
   </si>
   <si>
     <t>זוג גופיות חצי שרוול איכותיות בגיר - מידה 3XL</t>
+  </si>
+  <si>
+    <t>בדיקה שקד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בדיקה שקד2 </t>
+  </si>
+  <si>
+    <t>בדיקה שקד 3</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 5</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 4</t>
   </si>
 </sst>
 </file>
@@ -945,7 +960,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -1200,7 +1215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1301,6 +1316,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1588,8 +1609,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F56A6FD9-30DE-4534-9700-808734F282CD}" name="tbl_Familys" displayName="tbl_Familys" ref="A1:E291" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="A1:E291" xr:uid="{8781FA7B-3B84-43F7-B161-1EC7FB5AC567}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F56A6FD9-30DE-4534-9700-808734F282CD}" name="tbl_Familys" displayName="tbl_Familys" ref="A1:E296" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="A1:E296" xr:uid="{8781FA7B-3B84-43F7-B161-1EC7FB5AC567}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D2">
     <sortCondition ref="D1:D2"/>
   </sortState>
@@ -1605,7 +1626,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1922,23 +1943,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49E19-C7F0-4290-98E2-522667B31E5F}">
   <sheetPr codeName="גיליון8"/>
-  <dimension ref="A1:E291"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A282" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B296" sqref="B296"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1">
+    <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1">
+    <row r="2" spans="1:5" ht="17" thickBot="1">
       <c r="A2" s="2">
         <v>7304</v>
       </c>
@@ -1967,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1">
+    <row r="3" spans="1:5" ht="17" thickBot="1">
       <c r="A3" s="6">
         <v>907</v>
       </c>
@@ -1979,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1">
+    <row r="4" spans="1:5" ht="17" thickBot="1">
       <c r="A4" s="6">
         <v>5300</v>
       </c>
@@ -1991,7 +2012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1">
+    <row r="5" spans="1:5" ht="17" thickBot="1">
       <c r="A5" s="6">
         <v>831</v>
       </c>
@@ -2003,7 +2024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" thickBot="1">
+    <row r="6" spans="1:5" ht="17" thickBot="1">
       <c r="A6" s="9">
         <v>1853</v>
       </c>
@@ -2015,7 +2036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" thickBot="1">
+    <row r="7" spans="1:5" ht="17" thickBot="1">
       <c r="A7" s="9">
         <v>5306</v>
       </c>
@@ -2027,7 +2048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" thickBot="1">
+    <row r="8" spans="1:5" ht="17" thickBot="1">
       <c r="A8" s="9">
         <v>1833</v>
       </c>
@@ -2039,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1">
+    <row r="9" spans="1:5" ht="17" thickBot="1">
       <c r="A9" s="9">
         <v>1834</v>
       </c>
@@ -2051,7 +2072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" thickBot="1">
+    <row r="10" spans="1:5" ht="17" thickBot="1">
       <c r="A10" s="9">
         <v>6553</v>
       </c>
@@ -2063,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" thickBot="1">
+    <row r="11" spans="1:5" ht="17" thickBot="1">
       <c r="A11" s="9">
         <v>1835</v>
       </c>
@@ -2075,7 +2096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" thickBot="1">
+    <row r="12" spans="1:5" ht="17" thickBot="1">
       <c r="A12" s="9">
         <v>1836</v>
       </c>
@@ -2087,7 +2108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" thickBot="1">
+    <row r="13" spans="1:5" ht="17" thickBot="1">
       <c r="A13" s="9">
         <v>1837</v>
       </c>
@@ -2099,7 +2120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" thickBot="1">
+    <row r="14" spans="1:5" ht="17" thickBot="1">
       <c r="A14" s="9">
         <v>1838</v>
       </c>
@@ -2111,7 +2132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" thickBot="1">
+    <row r="15" spans="1:5" ht="17" thickBot="1">
       <c r="A15" s="9">
         <v>1839</v>
       </c>
@@ -2123,7 +2144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" thickBot="1">
+    <row r="16" spans="1:5" ht="17" thickBot="1">
       <c r="A16" s="9">
         <v>1840</v>
       </c>
@@ -2135,7 +2156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1">
+    <row r="17" spans="1:4" ht="17" thickBot="1">
       <c r="A17" s="9">
         <v>1841</v>
       </c>
@@ -2147,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" thickBot="1">
+    <row r="18" spans="1:4" ht="17" thickBot="1">
       <c r="A18" s="9">
         <v>1842</v>
       </c>
@@ -2159,7 +2180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1">
+    <row r="19" spans="1:4" ht="17" thickBot="1">
       <c r="A19" s="9">
         <v>1843</v>
       </c>
@@ -2171,7 +2192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1">
+    <row r="20" spans="1:4" ht="17" thickBot="1">
       <c r="A20" s="9">
         <v>1844</v>
       </c>
@@ -2183,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1">
+    <row r="21" spans="1:4" ht="17" thickBot="1">
       <c r="A21" s="9">
         <v>1845</v>
       </c>
@@ -2195,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1">
+    <row r="22" spans="1:4" ht="17" thickBot="1">
       <c r="A22" s="9">
         <v>1846</v>
       </c>
@@ -2207,7 +2228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1">
+    <row r="23" spans="1:4" ht="17" thickBot="1">
       <c r="A23" s="9">
         <v>1847</v>
       </c>
@@ -2219,7 +2240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" thickBot="1">
+    <row r="24" spans="1:4" ht="17" thickBot="1">
       <c r="A24" s="9">
         <v>1848</v>
       </c>
@@ -2231,7 +2252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1">
+    <row r="25" spans="1:4" ht="17" thickBot="1">
       <c r="A25" s="9">
         <v>1849</v>
       </c>
@@ -2243,7 +2264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1">
+    <row r="26" spans="1:4" ht="17" thickBot="1">
       <c r="A26" s="9">
         <v>1850</v>
       </c>
@@ -2255,7 +2276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1">
+    <row r="27" spans="1:4" ht="17" thickBot="1">
       <c r="A27" s="9">
         <v>1851</v>
       </c>
@@ -2267,7 +2288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1">
+    <row r="28" spans="1:4" ht="17" thickBot="1">
       <c r="A28" s="9">
         <v>1852</v>
       </c>
@@ -2279,7 +2300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1">
+    <row r="29" spans="1:4" ht="17" thickBot="1">
       <c r="A29" s="9">
         <v>5378</v>
       </c>
@@ -2291,7 +2312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" thickBot="1">
+    <row r="30" spans="1:4" ht="17" thickBot="1">
       <c r="A30" s="9">
         <v>5379</v>
       </c>
@@ -2303,7 +2324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" thickBot="1">
+    <row r="31" spans="1:4" ht="17" thickBot="1">
       <c r="A31" s="9">
         <v>6551</v>
       </c>
@@ -2315,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1">
+    <row r="32" spans="1:4" ht="17" thickBot="1">
       <c r="A32" s="9">
         <v>6552</v>
       </c>
@@ -2327,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" thickBot="1">
+    <row r="33" spans="1:4" ht="17" thickBot="1">
       <c r="A33" s="9">
         <v>6055</v>
       </c>
@@ -2339,7 +2360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" thickBot="1">
+    <row r="34" spans="1:4" ht="17" thickBot="1">
       <c r="A34" s="9">
         <v>6056</v>
       </c>
@@ -2351,7 +2372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" thickBot="1">
+    <row r="35" spans="1:4" ht="17" thickBot="1">
       <c r="A35" s="9">
         <v>6057</v>
       </c>
@@ -2363,7 +2384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" thickBot="1">
+    <row r="36" spans="1:4" ht="17" thickBot="1">
       <c r="A36" s="9">
         <v>6058</v>
       </c>
@@ -2375,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" thickBot="1">
+    <row r="37" spans="1:4" ht="17" thickBot="1">
       <c r="A37" s="9">
         <v>6059</v>
       </c>
@@ -2387,7 +2408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1">
+    <row r="38" spans="1:4" ht="17" thickBot="1">
       <c r="A38" s="9">
         <v>6060</v>
       </c>
@@ -2399,7 +2420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" thickBot="1">
+    <row r="39" spans="1:4" ht="17" thickBot="1">
       <c r="A39" s="9">
         <v>6061</v>
       </c>
@@ -2411,7 +2432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" thickBot="1">
+    <row r="40" spans="1:4" ht="17" thickBot="1">
       <c r="A40" s="9">
         <v>6062</v>
       </c>
@@ -2423,7 +2444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" thickBot="1">
+    <row r="41" spans="1:4" ht="17" thickBot="1">
       <c r="A41" s="9">
         <v>6063</v>
       </c>
@@ -2435,7 +2456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" thickBot="1">
+    <row r="42" spans="1:4" ht="17" thickBot="1">
       <c r="A42" s="9">
         <v>6064</v>
       </c>
@@ -2447,7 +2468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" thickBot="1">
+    <row r="43" spans="1:4" ht="17" thickBot="1">
       <c r="A43" s="9">
         <v>6065</v>
       </c>
@@ -2459,7 +2480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18" thickBot="1">
+    <row r="44" spans="1:4" ht="17" thickBot="1">
       <c r="A44" s="9">
         <v>6066</v>
       </c>
@@ -2471,7 +2492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18" thickBot="1">
+    <row r="45" spans="1:4" ht="17" thickBot="1">
       <c r="A45" s="9">
         <v>6067</v>
       </c>
@@ -2483,7 +2504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18" thickBot="1">
+    <row r="46" spans="1:4" ht="17" thickBot="1">
       <c r="A46" s="9">
         <v>6068</v>
       </c>
@@ -2495,7 +2516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18" thickBot="1">
+    <row r="47" spans="1:4" ht="17" thickBot="1">
       <c r="A47" s="9">
         <v>6069</v>
       </c>
@@ -2507,7 +2528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18" thickBot="1">
+    <row r="48" spans="1:4" ht="17" thickBot="1">
       <c r="A48" s="9">
         <v>6070</v>
       </c>
@@ -2519,7 +2540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18" thickBot="1">
+    <row r="49" spans="1:4" ht="17" thickBot="1">
       <c r="A49" s="6">
         <v>6071</v>
       </c>
@@ -2531,7 +2552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18" thickBot="1">
+    <row r="50" spans="1:4" ht="17" thickBot="1">
       <c r="A50" s="6">
         <v>2499</v>
       </c>
@@ -2543,7 +2564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18" thickBot="1">
+    <row r="51" spans="1:4" ht="17" thickBot="1">
       <c r="A51" s="6">
         <v>7847</v>
       </c>
@@ -2555,7 +2576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18" thickBot="1">
+    <row r="52" spans="1:4" ht="17" thickBot="1">
       <c r="A52" s="6">
         <v>7848</v>
       </c>
@@ -2567,7 +2588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18" thickBot="1">
+    <row r="53" spans="1:4" ht="17" thickBot="1">
       <c r="A53" s="6">
         <v>7849</v>
       </c>
@@ -2579,7 +2600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="18" thickBot="1">
+    <row r="54" spans="1:4" ht="17" thickBot="1">
       <c r="A54" s="6">
         <v>7850</v>
       </c>
@@ -2591,7 +2612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18" thickBot="1">
+    <row r="55" spans="1:4" ht="17" thickBot="1">
       <c r="A55" s="6">
         <v>7851</v>
       </c>
@@ -2603,7 +2624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="18" thickBot="1">
+    <row r="56" spans="1:4" ht="17" thickBot="1">
       <c r="A56" s="6">
         <v>7852</v>
       </c>
@@ -2615,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="18" thickBot="1">
+    <row r="57" spans="1:4" ht="17" thickBot="1">
       <c r="A57" s="6">
         <v>7853</v>
       </c>
@@ -2627,7 +2648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" thickBot="1">
+    <row r="58" spans="1:4" ht="17" thickBot="1">
       <c r="A58" s="6">
         <v>7854</v>
       </c>
@@ -2639,7 +2660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="18" thickBot="1">
+    <row r="59" spans="1:4" ht="17" thickBot="1">
       <c r="A59" s="6">
         <v>7855</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="18" thickBot="1">
+    <row r="60" spans="1:4" ht="17" thickBot="1">
       <c r="A60" s="6">
         <v>7856</v>
       </c>
@@ -2663,7 +2684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="18" thickBot="1">
+    <row r="61" spans="1:4" ht="17" thickBot="1">
       <c r="A61" s="6">
         <v>7857</v>
       </c>
@@ -2675,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18" thickBot="1">
+    <row r="62" spans="1:4" ht="17" thickBot="1">
       <c r="A62" s="6">
         <v>7858</v>
       </c>
@@ -2687,7 +2708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18" thickBot="1">
+    <row r="63" spans="1:4" ht="17" thickBot="1">
       <c r="A63" s="6">
         <v>7859</v>
       </c>
@@ -2699,7 +2720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="18" thickBot="1">
+    <row r="64" spans="1:4" ht="17" thickBot="1">
       <c r="A64" s="6">
         <v>7860</v>
       </c>
@@ -2711,7 +2732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18" thickBot="1">
+    <row r="65" spans="1:4" ht="17" thickBot="1">
       <c r="A65" s="6">
         <v>7861</v>
       </c>
@@ -2723,7 +2744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="18" thickBot="1">
+    <row r="66" spans="1:4" ht="17" thickBot="1">
       <c r="A66" s="6">
         <v>7862</v>
       </c>
@@ -2735,7 +2756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="18" thickBot="1">
+    <row r="67" spans="1:4" ht="17" thickBot="1">
       <c r="A67" s="6">
         <v>7863</v>
       </c>
@@ -2747,7 +2768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="18" thickBot="1">
+    <row r="68" spans="1:4" ht="17" thickBot="1">
       <c r="A68" s="6">
         <v>7864</v>
       </c>
@@ -2759,7 +2780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="18" thickBot="1">
+    <row r="69" spans="1:4" ht="17" thickBot="1">
       <c r="A69" s="6">
         <v>7865</v>
       </c>
@@ -2771,7 +2792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="18" thickBot="1">
+    <row r="70" spans="1:4" ht="17" thickBot="1">
       <c r="A70" s="6">
         <v>2498</v>
       </c>
@@ -2783,7 +2804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="18" thickBot="1">
+    <row r="71" spans="1:4" ht="17" thickBot="1">
       <c r="A71" s="6">
         <v>5304</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="18" thickBot="1">
+    <row r="72" spans="1:4" ht="17" thickBot="1">
       <c r="A72" s="6">
         <v>2030</v>
       </c>
@@ -2807,7 +2828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="18" thickBot="1">
+    <row r="73" spans="1:4" ht="17" thickBot="1">
       <c r="A73" s="6">
         <v>5837</v>
       </c>
@@ -2819,7 +2840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="18" thickBot="1">
+    <row r="74" spans="1:4" ht="17" thickBot="1">
       <c r="A74" s="6">
         <v>5617</v>
       </c>
@@ -2831,7 +2852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="18" thickBot="1">
+    <row r="75" spans="1:4" ht="17" thickBot="1">
       <c r="A75" s="6">
         <v>5384</v>
       </c>
@@ -2843,7 +2864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="18" thickBot="1">
+    <row r="76" spans="1:4" ht="17" thickBot="1">
       <c r="A76" s="6">
         <v>5753</v>
       </c>
@@ -2855,7 +2876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="18" thickBot="1">
+    <row r="77" spans="1:4" ht="17" thickBot="1">
       <c r="A77" s="6">
         <v>6164</v>
       </c>
@@ -2867,7 +2888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="18" thickBot="1">
+    <row r="78" spans="1:4" ht="17" thickBot="1">
       <c r="A78" s="6">
         <v>5383</v>
       </c>
@@ -2879,7 +2900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18" thickBot="1">
+    <row r="79" spans="1:4" ht="17" thickBot="1">
       <c r="A79" s="6">
         <v>5754</v>
       </c>
@@ -2891,7 +2912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="18" thickBot="1">
+    <row r="80" spans="1:4" ht="17" thickBot="1">
       <c r="A80" s="13">
         <v>2380</v>
       </c>
@@ -2903,7 +2924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="18" thickBot="1">
+    <row r="81" spans="1:4" ht="17" thickBot="1">
       <c r="A81" s="13">
         <v>2381</v>
       </c>
@@ -2915,7 +2936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18" thickBot="1">
+    <row r="82" spans="1:4" ht="17" thickBot="1">
       <c r="A82" s="13">
         <v>2382</v>
       </c>
@@ -2927,7 +2948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="18" thickBot="1">
+    <row r="83" spans="1:4" ht="17" thickBot="1">
       <c r="A83" s="13">
         <v>2383</v>
       </c>
@@ -2939,7 +2960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="18" thickBot="1">
+    <row r="84" spans="1:4" ht="17" thickBot="1">
       <c r="A84" s="9">
         <v>5609</v>
       </c>
@@ -2951,7 +2972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18" thickBot="1">
+    <row r="85" spans="1:4" ht="17" thickBot="1">
       <c r="A85" s="9">
         <v>5610</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="18" thickBot="1">
+    <row r="86" spans="1:4" ht="17" thickBot="1">
       <c r="A86" s="13">
         <v>5611</v>
       </c>
@@ -2975,7 +2996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="18" thickBot="1">
+    <row r="87" spans="1:4" ht="17" thickBot="1">
       <c r="A87" s="13">
         <v>5612</v>
       </c>
@@ -2987,7 +3008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="18" thickBot="1">
+    <row r="88" spans="1:4" ht="17" thickBot="1">
       <c r="A88" s="13">
         <v>5613</v>
       </c>
@@ -2999,7 +3020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18" thickBot="1">
+    <row r="89" spans="1:4" ht="17" thickBot="1">
       <c r="A89" s="13">
         <v>5614</v>
       </c>
@@ -3011,7 +3032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="18" thickBot="1">
+    <row r="90" spans="1:4" ht="17" thickBot="1">
       <c r="A90" s="13">
         <v>5615</v>
       </c>
@@ -3023,7 +3044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="18" thickBot="1">
+    <row r="91" spans="1:4" ht="17" thickBot="1">
       <c r="A91" s="13">
         <v>5616</v>
       </c>
@@ -3035,7 +3056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="18" thickBot="1">
+    <row r="92" spans="1:4" ht="17" thickBot="1">
       <c r="A92" s="6">
         <v>7313</v>
       </c>
@@ -3047,7 +3068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="18" thickBot="1">
+    <row r="93" spans="1:4" ht="17" thickBot="1">
       <c r="A93" s="6">
         <v>7312</v>
       </c>
@@ -3059,7 +3080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="18" thickBot="1">
+    <row r="94" spans="1:4" ht="17" thickBot="1">
       <c r="A94" s="6">
         <v>7314</v>
       </c>
@@ -3071,7 +3092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="18" thickBot="1">
+    <row r="95" spans="1:4" ht="17" thickBot="1">
       <c r="A95" s="6">
         <v>7315</v>
       </c>
@@ -3083,7 +3104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="18" thickBot="1">
+    <row r="96" spans="1:4" ht="17" thickBot="1">
       <c r="A96" s="13">
         <v>7976</v>
       </c>
@@ -3095,7 +3116,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="18" thickBot="1">
+    <row r="97" spans="1:4" ht="17" thickBot="1">
       <c r="A97" s="13">
         <v>7977</v>
       </c>
@@ -3107,7 +3128,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="18" thickBot="1">
+    <row r="98" spans="1:4" ht="17" thickBot="1">
       <c r="A98" s="13">
         <v>7978</v>
       </c>
@@ -3119,7 +3140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="18" thickBot="1">
+    <row r="99" spans="1:4" ht="17" thickBot="1">
       <c r="A99" s="13">
         <v>7979</v>
       </c>
@@ -3131,7 +3152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="18" thickBot="1">
+    <row r="100" spans="1:4" ht="17" thickBot="1">
       <c r="A100" s="13">
         <v>2234</v>
       </c>
@@ -3143,7 +3164,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="18" thickBot="1">
+    <row r="101" spans="1:4" ht="17" thickBot="1">
       <c r="A101" s="13">
         <v>2235</v>
       </c>
@@ -3155,7 +3176,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="18" thickBot="1">
+    <row r="102" spans="1:4" ht="17" thickBot="1">
       <c r="A102" s="13">
         <v>2236</v>
       </c>
@@ -3167,7 +3188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="18" thickBot="1">
+    <row r="103" spans="1:4" ht="17" thickBot="1">
       <c r="A103" s="13">
         <v>2237</v>
       </c>
@@ -3179,7 +3200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="18" thickBot="1">
+    <row r="104" spans="1:4" ht="17" thickBot="1">
       <c r="A104" s="13">
         <v>2238</v>
       </c>
@@ -3191,7 +3212,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="18" thickBot="1">
+    <row r="105" spans="1:4" ht="17" thickBot="1">
       <c r="A105" s="13">
         <v>6406</v>
       </c>
@@ -3203,7 +3224,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="18" thickBot="1">
+    <row r="106" spans="1:4" ht="17" thickBot="1">
       <c r="A106" s="6">
         <v>7980</v>
       </c>
@@ -3215,7 +3236,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="18" thickBot="1">
+    <row r="107" spans="1:4" ht="17" thickBot="1">
       <c r="A107" s="13">
         <v>7885</v>
       </c>
@@ -3227,7 +3248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="18" thickBot="1">
+    <row r="108" spans="1:4" ht="17" thickBot="1">
       <c r="A108" s="13">
         <v>7886</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="18" thickBot="1">
+    <row r="109" spans="1:4" ht="17" thickBot="1">
       <c r="A109" s="13">
         <v>7887</v>
       </c>
@@ -3251,7 +3272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="18" thickBot="1">
+    <row r="110" spans="1:4" ht="17" thickBot="1">
       <c r="A110" s="13">
         <v>7888</v>
       </c>
@@ -3263,7 +3284,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="18" thickBot="1">
+    <row r="111" spans="1:4" ht="17" thickBot="1">
       <c r="A111" s="13">
         <v>7889</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="18" thickBot="1">
+    <row r="112" spans="1:4" ht="17" thickBot="1">
       <c r="A112" s="13">
         <v>7890</v>
       </c>
@@ -3287,7 +3308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="18" thickBot="1">
+    <row r="113" spans="1:4" ht="17" thickBot="1">
       <c r="A113" s="6">
         <v>5978</v>
       </c>
@@ -3299,7 +3320,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="18" thickBot="1">
+    <row r="114" spans="1:4" ht="17" thickBot="1">
       <c r="A114" s="6">
         <v>5979</v>
       </c>
@@ -3311,7 +3332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="18" thickBot="1">
+    <row r="115" spans="1:4" ht="17" thickBot="1">
       <c r="A115" s="6">
         <v>5980</v>
       </c>
@@ -3323,7 +3344,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="18" thickBot="1">
+    <row r="116" spans="1:4" ht="17" thickBot="1">
       <c r="A116" s="6">
         <v>5981</v>
       </c>
@@ -3335,7 +3356,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="18" thickBot="1">
+    <row r="117" spans="1:4" ht="17" thickBot="1">
       <c r="A117" s="6">
         <v>5982</v>
       </c>
@@ -3347,7 +3368,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="18" thickBot="1">
+    <row r="118" spans="1:4" ht="17" thickBot="1">
       <c r="A118" s="6">
         <v>5983</v>
       </c>
@@ -3359,7 +3380,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="18" thickBot="1">
+    <row r="119" spans="1:4" ht="17" thickBot="1">
       <c r="A119" s="13">
         <v>7770</v>
       </c>
@@ -3371,7 +3392,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="18" thickBot="1">
+    <row r="120" spans="1:4" ht="17" thickBot="1">
       <c r="A120" s="13">
         <v>7772</v>
       </c>
@@ -3383,7 +3404,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="18" thickBot="1">
+    <row r="121" spans="1:4" ht="17" thickBot="1">
       <c r="A121" s="13">
         <v>7773</v>
       </c>
@@ -3395,7 +3416,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="18" thickBot="1">
+    <row r="122" spans="1:4" ht="17" thickBot="1">
       <c r="A122" s="6">
         <v>7964</v>
       </c>
@@ -3407,7 +3428,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="18" thickBot="1">
+    <row r="123" spans="1:4" ht="17" thickBot="1">
       <c r="A123" s="6">
         <v>5145</v>
       </c>
@@ -3419,7 +3440,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="18" thickBot="1">
+    <row r="124" spans="1:4" ht="17" thickBot="1">
       <c r="A124" s="6">
         <v>5141</v>
       </c>
@@ -3431,7 +3452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="18" thickBot="1">
+    <row r="125" spans="1:4" ht="17" thickBot="1">
       <c r="A125" s="6">
         <v>5142</v>
       </c>
@@ -3443,7 +3464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="18" thickBot="1">
+    <row r="126" spans="1:4" ht="17" thickBot="1">
       <c r="A126" s="6">
         <v>5143</v>
       </c>
@@ -3455,7 +3476,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="18" thickBot="1">
+    <row r="127" spans="1:4" ht="17" thickBot="1">
       <c r="A127" s="6">
         <v>5144</v>
       </c>
@@ -3467,7 +3488,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="18" thickBot="1">
+    <row r="128" spans="1:4" ht="17" thickBot="1">
       <c r="A128" s="6">
         <v>5836</v>
       </c>
@@ -3479,7 +3500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="18" thickBot="1">
+    <row r="129" spans="1:4" ht="17" thickBot="1">
       <c r="A129" s="6">
         <v>8156</v>
       </c>
@@ -3491,7 +3512,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="18" thickBot="1">
+    <row r="130" spans="1:4" ht="17" thickBot="1">
       <c r="A130" s="6">
         <v>8157</v>
       </c>
@@ -3503,7 +3524,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="18" thickBot="1">
+    <row r="131" spans="1:4" ht="17" thickBot="1">
       <c r="A131" s="9">
         <v>2449</v>
       </c>
@@ -3515,7 +3536,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="18" thickBot="1">
+    <row r="132" spans="1:4" ht="17" thickBot="1">
       <c r="A132" s="6">
         <v>8159</v>
       </c>
@@ -3527,7 +3548,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="18" thickBot="1">
+    <row r="133" spans="1:4" ht="17" thickBot="1">
       <c r="A133" s="6">
         <v>8160</v>
       </c>
@@ -3539,7 +3560,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="18" thickBot="1">
+    <row r="134" spans="1:4" ht="17" thickBot="1">
       <c r="A134" s="6">
         <v>8161</v>
       </c>
@@ -3551,7 +3572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="18" thickBot="1">
+    <row r="135" spans="1:4" ht="17" thickBot="1">
       <c r="A135" s="9">
         <v>8099</v>
       </c>
@@ -3563,7 +3584,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="18" thickBot="1">
+    <row r="136" spans="1:4" ht="17" thickBot="1">
       <c r="A136" s="9">
         <v>8083</v>
       </c>
@@ -3575,7 +3596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="18" thickBot="1">
+    <row r="137" spans="1:4" ht="17" thickBot="1">
       <c r="A137" s="9">
         <v>8141</v>
       </c>
@@ -3587,7 +3608,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="18" thickBot="1">
+    <row r="138" spans="1:4" ht="17" thickBot="1">
       <c r="A138" s="9">
         <v>8139</v>
       </c>
@@ -3599,7 +3620,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="18" thickBot="1">
+    <row r="139" spans="1:4" ht="17" thickBot="1">
       <c r="A139" s="9">
         <v>8142</v>
       </c>
@@ -3611,7 +3632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="18" thickBot="1">
+    <row r="140" spans="1:4" ht="17" thickBot="1">
       <c r="A140" s="18">
         <v>8081</v>
       </c>
@@ -3623,7 +3644,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="18" thickBot="1">
+    <row r="141" spans="1:4" ht="17" thickBot="1">
       <c r="A141" s="18">
         <v>8082</v>
       </c>
@@ -3635,7 +3656,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="18" thickBot="1">
+    <row r="142" spans="1:4" ht="17" thickBot="1">
       <c r="A142" s="18">
         <v>8084</v>
       </c>
@@ -3647,7 +3668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="18" thickBot="1">
+    <row r="143" spans="1:4" ht="17" thickBot="1">
       <c r="A143" s="5">
         <v>8140</v>
       </c>
@@ -3659,7 +3680,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="18" thickBot="1">
+    <row r="144" spans="1:4" ht="17" thickBot="1">
       <c r="A144" s="5">
         <v>8138</v>
       </c>
@@ -3671,7 +3692,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="18" thickBot="1">
+    <row r="145" spans="1:4" ht="17" thickBot="1">
       <c r="A145" s="5">
         <v>8080</v>
       </c>
@@ -3683,7 +3704,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="18" thickBot="1">
+    <row r="146" spans="1:4" ht="17" thickBot="1">
       <c r="A146" s="5">
         <v>8137</v>
       </c>
@@ -3695,7 +3716,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="18" thickBot="1">
+    <row r="147" spans="1:4" ht="17" thickBot="1">
       <c r="A147" s="5">
         <v>8079</v>
       </c>
@@ -3707,7 +3728,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="18" thickBot="1">
+    <row r="148" spans="1:4" ht="17" thickBot="1">
       <c r="A148" s="5">
         <v>7305</v>
       </c>
@@ -3719,7 +3740,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="18" thickBot="1">
+    <row r="149" spans="1:4" ht="17" thickBot="1">
       <c r="A149" s="5">
         <v>7307</v>
       </c>
@@ -3731,7 +3752,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="18" thickBot="1">
+    <row r="150" spans="1:4" ht="17" thickBot="1">
       <c r="A150" s="5">
         <v>7634</v>
       </c>
@@ -3743,7 +3764,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="18" thickBot="1">
+    <row r="151" spans="1:4" ht="17" thickBot="1">
       <c r="A151" s="5">
         <v>7765</v>
       </c>
@@ -3755,7 +3776,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="18" thickBot="1">
+    <row r="152" spans="1:4" ht="17" thickBot="1">
       <c r="A152" s="5">
         <v>7884</v>
       </c>
@@ -3767,7 +3788,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="18" thickBot="1">
+    <row r="153" spans="1:4" ht="17" thickBot="1">
       <c r="A153" s="19">
         <v>5835</v>
       </c>
@@ -3779,7 +3800,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="18" thickBot="1">
+    <row r="154" spans="1:4" ht="17" thickBot="1">
       <c r="A154" s="19">
         <v>1948</v>
       </c>
@@ -3791,7 +3812,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="18" thickBot="1">
+    <row r="155" spans="1:4" ht="17" thickBot="1">
       <c r="A155" s="19">
         <v>7755</v>
       </c>
@@ -3803,7 +3824,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="18" thickBot="1">
+    <row r="156" spans="1:4" ht="17" thickBot="1">
       <c r="A156" s="22">
         <v>1942</v>
       </c>
@@ -3815,7 +3836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="18" thickBot="1">
+    <row r="157" spans="1:4" ht="17" thickBot="1">
       <c r="A157" s="22">
         <v>1943</v>
       </c>
@@ -3827,7 +3848,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="18" thickBot="1">
+    <row r="158" spans="1:4" ht="17" thickBot="1">
       <c r="A158" s="22">
         <v>1944</v>
       </c>
@@ -3839,7 +3860,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="18" thickBot="1">
+    <row r="159" spans="1:4" ht="17" thickBot="1">
       <c r="A159" s="22">
         <v>2384</v>
       </c>
@@ -3851,7 +3872,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="18" thickBot="1">
+    <row r="160" spans="1:4" ht="17" thickBot="1">
       <c r="A160" s="22">
         <v>2385</v>
       </c>
@@ -3863,7 +3884,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="18" thickBot="1">
+    <row r="161" spans="1:4" ht="17" thickBot="1">
       <c r="A161" s="22">
         <v>2460</v>
       </c>
@@ -3875,7 +3896,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="18" thickBot="1">
+    <row r="162" spans="1:4" ht="17" thickBot="1">
       <c r="A162" s="22">
         <v>5020</v>
       </c>
@@ -3887,7 +3908,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="18" thickBot="1">
+    <row r="163" spans="1:4" ht="17" thickBot="1">
       <c r="A163" s="22">
         <v>5377</v>
       </c>
@@ -3899,7 +3920,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="18" thickBot="1">
+    <row r="164" spans="1:4" ht="17" thickBot="1">
       <c r="A164" s="22">
         <v>2075</v>
       </c>
@@ -3911,7 +3932,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="18" thickBot="1">
+    <row r="165" spans="1:4" ht="17" thickBot="1">
       <c r="A165" s="22">
         <v>1928</v>
       </c>
@@ -3923,7 +3944,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="18" thickBot="1">
+    <row r="166" spans="1:4" ht="17" thickBot="1">
       <c r="A166" s="22">
         <v>1929</v>
       </c>
@@ -3935,7 +3956,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="18" thickBot="1">
+    <row r="167" spans="1:4" ht="17" thickBot="1">
       <c r="A167" s="22">
         <v>1930</v>
       </c>
@@ -3947,7 +3968,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="18" thickBot="1">
+    <row r="168" spans="1:4" ht="17" thickBot="1">
       <c r="A168" s="22">
         <v>1933</v>
       </c>
@@ -3959,7 +3980,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="18" thickBot="1">
+    <row r="169" spans="1:4" ht="17" thickBot="1">
       <c r="A169" s="22">
         <v>1934</v>
       </c>
@@ -3971,7 +3992,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="18" thickBot="1">
+    <row r="170" spans="1:4" ht="17" thickBot="1">
       <c r="A170" s="22">
         <v>1931</v>
       </c>
@@ -3983,7 +4004,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="18" thickBot="1">
+    <row r="171" spans="1:4" ht="17" thickBot="1">
       <c r="A171" s="22">
         <v>1932</v>
       </c>
@@ -3995,7 +4016,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="18" thickBot="1">
+    <row r="172" spans="1:4" ht="17" thickBot="1">
       <c r="A172" s="22">
         <v>6407</v>
       </c>
@@ -4007,7 +4028,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="18" thickBot="1">
+    <row r="173" spans="1:4" ht="17" thickBot="1">
       <c r="A173" s="22">
         <v>784</v>
       </c>
@@ -4019,7 +4040,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="18" thickBot="1">
+    <row r="174" spans="1:4" ht="17" thickBot="1">
       <c r="A174" s="22">
         <v>1953</v>
       </c>
@@ -4031,7 +4052,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="18" thickBot="1">
+    <row r="175" spans="1:4" ht="17" thickBot="1">
       <c r="A175" s="22">
         <v>1950</v>
       </c>
@@ -4043,7 +4064,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="18" thickBot="1">
+    <row r="176" spans="1:4" ht="17" thickBot="1">
       <c r="A176" s="22">
         <v>1951</v>
       </c>
@@ -4055,7 +4076,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="18" thickBot="1">
+    <row r="177" spans="1:4" ht="17" thickBot="1">
       <c r="A177" s="22">
         <v>1952</v>
       </c>
@@ -4067,7 +4088,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="18" thickBot="1">
+    <row r="178" spans="1:4" ht="17" thickBot="1">
       <c r="A178" s="23">
         <v>2031</v>
       </c>
@@ -4079,7 +4100,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="18" thickBot="1">
+    <row r="179" spans="1:4" ht="17" thickBot="1">
       <c r="A179" s="9">
         <v>2461</v>
       </c>
@@ -4091,7 +4112,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="18" thickBot="1">
+    <row r="180" spans="1:4" ht="17" thickBot="1">
       <c r="A180" s="23">
         <v>6517</v>
       </c>
@@ -4103,7 +4124,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="18" thickBot="1">
+    <row r="181" spans="1:4" ht="17" thickBot="1">
       <c r="A181" s="22">
         <v>6705</v>
       </c>
@@ -4115,7 +4136,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="18" thickBot="1">
+    <row r="182" spans="1:4" ht="17" thickBot="1">
       <c r="A182" s="26">
         <v>2032</v>
       </c>
@@ -4127,7 +4148,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="18" thickBot="1">
+    <row r="183" spans="1:4" ht="17" thickBot="1">
       <c r="A183" s="26">
         <v>2033</v>
       </c>
@@ -4139,7 +4160,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="18" thickBot="1">
+    <row r="184" spans="1:4" ht="17" thickBot="1">
       <c r="A184" s="26">
         <v>750</v>
       </c>
@@ -4151,7 +4172,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="18" thickBot="1">
+    <row r="185" spans="1:4" ht="17" thickBot="1">
       <c r="A185" s="26">
         <v>2074</v>
       </c>
@@ -4163,7 +4184,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="18" thickBot="1">
+    <row r="186" spans="1:4" ht="17" thickBot="1">
       <c r="A186" s="26">
         <v>1937</v>
       </c>
@@ -4175,7 +4196,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="18" thickBot="1">
+    <row r="187" spans="1:4" ht="17" thickBot="1">
       <c r="A187" s="26">
         <v>1935</v>
       </c>
@@ -4187,7 +4208,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="18" thickBot="1">
+    <row r="188" spans="1:4" ht="17" thickBot="1">
       <c r="A188" s="26">
         <v>1936</v>
       </c>
@@ -4199,7 +4220,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="18" thickBot="1">
+    <row r="189" spans="1:4" ht="17" thickBot="1">
       <c r="A189" s="26">
         <v>1938</v>
       </c>
@@ -4211,7 +4232,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="18" thickBot="1">
+    <row r="190" spans="1:4" ht="17" thickBot="1">
       <c r="A190" s="26">
         <v>1939</v>
       </c>
@@ -4223,7 +4244,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="18" thickBot="1">
+    <row r="191" spans="1:4" ht="17" thickBot="1">
       <c r="A191" s="22">
         <v>1940</v>
       </c>
@@ -4235,7 +4256,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="18" thickBot="1">
+    <row r="192" spans="1:4" ht="17" thickBot="1">
       <c r="A192" s="22">
         <v>1941</v>
       </c>
@@ -4247,7 +4268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="18" thickBot="1">
+    <row r="193" spans="1:4" ht="17" thickBot="1">
       <c r="A193" s="22">
         <v>6536</v>
       </c>
@@ -4259,7 +4280,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="18" thickBot="1">
+    <row r="194" spans="1:4" ht="17" thickBot="1">
       <c r="A194" s="22">
         <v>5149</v>
       </c>
@@ -4271,7 +4292,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="18" thickBot="1">
+    <row r="195" spans="1:4" ht="17" thickBot="1">
       <c r="A195" s="22">
         <v>5150</v>
       </c>
@@ -4283,7 +4304,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="18" thickBot="1">
+    <row r="196" spans="1:4" ht="17" thickBot="1">
       <c r="A196" s="22">
         <v>5151</v>
       </c>
@@ -4295,7 +4316,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="18" thickBot="1">
+    <row r="197" spans="1:4" ht="17" thickBot="1">
       <c r="A197" s="22">
         <v>5152</v>
       </c>
@@ -4307,7 +4328,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="18" thickBot="1">
+    <row r="198" spans="1:4" ht="17" thickBot="1">
       <c r="A198" s="22">
         <v>5153</v>
       </c>
@@ -4319,7 +4340,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="18" thickBot="1">
+    <row r="199" spans="1:4" ht="17" thickBot="1">
       <c r="A199" s="22">
         <v>5376</v>
       </c>
@@ -4331,7 +4352,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="18" thickBot="1">
+    <row r="200" spans="1:4" ht="17" thickBot="1">
       <c r="A200" s="19">
         <v>5310</v>
       </c>
@@ -4343,7 +4364,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="18" thickBot="1">
+    <row r="201" spans="1:4" ht="17" thickBot="1">
       <c r="A201" s="19">
         <v>7015</v>
       </c>
@@ -4355,7 +4376,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="18" thickBot="1">
+    <row r="202" spans="1:4" ht="17" thickBot="1">
       <c r="A202" s="25">
         <v>7016</v>
       </c>
@@ -4367,7 +4388,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="18" thickBot="1">
+    <row r="203" spans="1:4" ht="17" thickBot="1">
       <c r="A203" s="19">
         <v>7017</v>
       </c>
@@ -4379,7 +4400,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="18" thickBot="1">
+    <row r="204" spans="1:4" ht="17" thickBot="1">
       <c r="A204" s="19">
         <v>7018</v>
       </c>
@@ -4391,7 +4412,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="18" thickBot="1">
+    <row r="205" spans="1:4" ht="17" thickBot="1">
       <c r="A205" s="19">
         <v>7019</v>
       </c>
@@ -4403,7 +4424,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="18" thickBot="1">
+    <row r="206" spans="1:4" ht="17" thickBot="1">
       <c r="A206" s="19">
         <v>7020</v>
       </c>
@@ -4415,7 +4436,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="18" thickBot="1">
+    <row r="207" spans="1:4" ht="17" thickBot="1">
       <c r="A207" s="19">
         <v>7021</v>
       </c>
@@ -4427,7 +4448,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="18" thickBot="1">
+    <row r="208" spans="1:4" ht="17" thickBot="1">
       <c r="A208" s="19">
         <v>1922</v>
       </c>
@@ -4439,7 +4460,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="18" thickBot="1">
+    <row r="209" spans="1:4" ht="17" thickBot="1">
       <c r="A209" s="19">
         <v>1923</v>
       </c>
@@ -4451,7 +4472,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="18" thickBot="1">
+    <row r="210" spans="1:4" ht="17" thickBot="1">
       <c r="A210" s="19">
         <v>1924</v>
       </c>
@@ -4463,7 +4484,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="18" thickBot="1">
+    <row r="211" spans="1:4" ht="17" thickBot="1">
       <c r="A211" s="19">
         <v>1925</v>
       </c>
@@ -4475,7 +4496,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="18" thickBot="1">
+    <row r="212" spans="1:4" ht="17" thickBot="1">
       <c r="A212" s="19">
         <v>1926</v>
       </c>
@@ -4487,7 +4508,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="18" thickBot="1">
+    <row r="213" spans="1:4" ht="17" thickBot="1">
       <c r="A213" s="19">
         <v>1927</v>
       </c>
@@ -4499,7 +4520,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="18" thickBot="1">
+    <row r="214" spans="1:4" ht="17" thickBot="1">
       <c r="A214" s="19">
         <v>2091</v>
       </c>
@@ -4511,7 +4532,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="18" thickBot="1">
+    <row r="215" spans="1:4" ht="17" thickBot="1">
       <c r="A215" s="19">
         <v>2077</v>
       </c>
@@ -4523,7 +4544,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="18" thickBot="1">
+    <row r="216" spans="1:4" ht="17" thickBot="1">
       <c r="A216" s="19">
         <v>2078</v>
       </c>
@@ -4535,7 +4556,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="18" thickBot="1">
+    <row r="217" spans="1:4" ht="17" thickBot="1">
       <c r="A217" s="19">
         <v>2079</v>
       </c>
@@ -4547,7 +4568,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="18" thickBot="1">
+    <row r="218" spans="1:4" ht="17" thickBot="1">
       <c r="A218" s="19">
         <v>2080</v>
       </c>
@@ -4559,7 +4580,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="18" thickBot="1">
+    <row r="219" spans="1:4" ht="17" thickBot="1">
       <c r="A219" s="19">
         <v>2081</v>
       </c>
@@ -4571,7 +4592,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="18" thickBot="1">
+    <row r="220" spans="1:4" ht="17" thickBot="1">
       <c r="A220" s="20">
         <v>7299</v>
       </c>
@@ -4583,7 +4604,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="18" thickBot="1">
+    <row r="221" spans="1:4" ht="17" thickBot="1">
       <c r="A221" s="19">
         <v>7429</v>
       </c>
@@ -4595,7 +4616,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="18" thickBot="1">
+    <row r="222" spans="1:4" ht="17" thickBot="1">
       <c r="A222" s="19">
         <v>7430</v>
       </c>
@@ -4607,7 +4628,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="18" thickBot="1">
+    <row r="223" spans="1:4" ht="17" thickBot="1">
       <c r="A223" s="19">
         <v>7431</v>
       </c>
@@ -4619,7 +4640,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="18" thickBot="1">
+    <row r="224" spans="1:4" ht="17" thickBot="1">
       <c r="A224" s="19">
         <v>7432</v>
       </c>
@@ -4631,7 +4652,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="18" thickBot="1">
+    <row r="225" spans="1:4" ht="17" thickBot="1">
       <c r="A225" s="19">
         <v>7435</v>
       </c>
@@ -4643,7 +4664,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="18" thickBot="1">
+    <row r="226" spans="1:4" ht="17" thickBot="1">
       <c r="A226" s="19">
         <v>7436</v>
       </c>
@@ -4655,7 +4676,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="18" thickBot="1">
+    <row r="227" spans="1:4" ht="17" thickBot="1">
       <c r="A227" s="19">
         <v>7437</v>
       </c>
@@ -4667,7 +4688,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="18" thickBot="1">
+    <row r="228" spans="1:4" ht="17" thickBot="1">
       <c r="A228" s="19">
         <v>7438</v>
       </c>
@@ -4679,7 +4700,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="18" thickBot="1">
+    <row r="229" spans="1:4" ht="17" thickBot="1">
       <c r="A229" s="19">
         <v>7439</v>
       </c>
@@ -4691,7 +4712,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="18" thickBot="1">
+    <row r="230" spans="1:4" ht="17" thickBot="1">
       <c r="A230" s="19">
         <v>7440</v>
       </c>
@@ -4703,7 +4724,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="18" thickBot="1">
+    <row r="231" spans="1:4" ht="17" thickBot="1">
       <c r="A231" s="19">
         <v>8312</v>
       </c>
@@ -4715,7 +4736,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="18" thickBot="1">
+    <row r="232" spans="1:4" ht="17" thickBot="1">
       <c r="A232" s="19">
         <v>8313</v>
       </c>
@@ -4727,7 +4748,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="18" thickBot="1">
+    <row r="233" spans="1:4" ht="17" thickBot="1">
       <c r="A233" s="19">
         <v>8314</v>
       </c>
@@ -4739,7 +4760,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="18" thickBot="1">
+    <row r="234" spans="1:4" ht="17" thickBot="1">
       <c r="A234" s="19">
         <v>2402</v>
       </c>
@@ -4751,7 +4772,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="18" thickBot="1">
+    <row r="235" spans="1:4" ht="17" thickBot="1">
       <c r="A235" s="19">
         <v>2403</v>
       </c>
@@ -4763,7 +4784,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="18" thickBot="1">
+    <row r="236" spans="1:4" ht="17" thickBot="1">
       <c r="A236" s="19">
         <v>2404</v>
       </c>
@@ -4775,7 +4796,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="18" thickBot="1">
+    <row r="237" spans="1:4" ht="17" thickBot="1">
       <c r="A237" s="19">
         <v>2405</v>
       </c>
@@ -4787,7 +4808,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="18" thickBot="1">
+    <row r="238" spans="1:4" ht="17" thickBot="1">
       <c r="A238" s="19">
         <v>5302</v>
       </c>
@@ -4799,7 +4820,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="18" thickBot="1">
+    <row r="239" spans="1:4" ht="17" thickBot="1">
       <c r="A239" s="19">
         <v>7303</v>
       </c>
@@ -4811,7 +4832,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="18" thickBot="1">
+    <row r="240" spans="1:4" ht="17" thickBot="1">
       <c r="A240" s="13">
         <v>2199</v>
       </c>
@@ -4823,7 +4844,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="18" thickBot="1">
+    <row r="241" spans="1:4" ht="17" thickBot="1">
       <c r="A241" s="13">
         <v>2200</v>
       </c>
@@ -4835,7 +4856,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="18" thickBot="1">
+    <row r="242" spans="1:4" ht="17" thickBot="1">
       <c r="A242" s="13">
         <v>2201</v>
       </c>
@@ -4847,7 +4868,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="18" thickBot="1">
+    <row r="243" spans="1:4" ht="17" thickBot="1">
       <c r="A243" s="13">
         <v>2202</v>
       </c>
@@ -4859,7 +4880,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="18" thickBot="1">
+    <row r="244" spans="1:4" ht="17" thickBot="1">
       <c r="A244" s="13">
         <v>2203</v>
       </c>
@@ -4871,7 +4892,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="18" thickBot="1">
+    <row r="245" spans="1:4" ht="17" thickBot="1">
       <c r="A245" s="13">
         <v>5162</v>
       </c>
@@ -4883,7 +4904,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="18" thickBot="1">
+    <row r="246" spans="1:4" ht="17" thickBot="1">
       <c r="A246" s="19">
         <v>7175</v>
       </c>
@@ -4895,7 +4916,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="18" thickBot="1">
+    <row r="247" spans="1:4" ht="17" thickBot="1">
       <c r="A247" s="19">
         <v>7211</v>
       </c>
@@ -4907,7 +4928,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="18" thickBot="1">
+    <row r="248" spans="1:4" ht="17" thickBot="1">
       <c r="A248" s="19">
         <v>7604</v>
       </c>
@@ -4919,7 +4940,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="18" thickBot="1">
+    <row r="249" spans="1:4" ht="17" thickBot="1">
       <c r="A249" s="19">
         <v>7564</v>
       </c>
@@ -4931,7 +4952,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="18" thickBot="1">
+    <row r="250" spans="1:4" ht="17" thickBot="1">
       <c r="A250" s="19">
         <v>7565</v>
       </c>
@@ -4943,7 +4964,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="18" thickBot="1">
+    <row r="251" spans="1:4" ht="17" thickBot="1">
       <c r="A251" s="19">
         <v>7566</v>
       </c>
@@ -4955,7 +4976,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="18" thickBot="1">
+    <row r="252" spans="1:4" ht="17" thickBot="1">
       <c r="A252" s="19">
         <v>7290</v>
       </c>
@@ -4967,7 +4988,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="18" thickBot="1">
+    <row r="253" spans="1:4" ht="17" thickBot="1">
       <c r="A253" s="19">
         <v>7295</v>
       </c>
@@ -4979,7 +5000,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="18" thickBot="1">
+    <row r="254" spans="1:4" ht="17" thickBot="1">
       <c r="A254" s="19">
         <v>7180</v>
       </c>
@@ -4991,7 +5012,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="18" thickBot="1">
+    <row r="255" spans="1:4" ht="17" thickBot="1">
       <c r="A255" s="19">
         <v>7181</v>
       </c>
@@ -5003,7 +5024,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="18" thickBot="1">
+    <row r="256" spans="1:4" ht="17" thickBot="1">
       <c r="A256" s="19">
         <v>7182</v>
       </c>
@@ -5015,7 +5036,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="18" thickBot="1">
+    <row r="257" spans="1:4" ht="17" thickBot="1">
       <c r="A257" s="19">
         <v>7183</v>
       </c>
@@ -5027,7 +5048,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="18" thickBot="1">
+    <row r="258" spans="1:4" ht="17" thickBot="1">
       <c r="A258" s="19">
         <v>7184</v>
       </c>
@@ -5039,7 +5060,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="18" thickBot="1">
+    <row r="259" spans="1:4" ht="17" thickBot="1">
       <c r="A259" s="19">
         <v>7185</v>
       </c>
@@ -5051,7 +5072,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="18" thickBot="1">
+    <row r="260" spans="1:4" ht="17" thickBot="1">
       <c r="A260" s="19">
         <v>7186</v>
       </c>
@@ -5063,7 +5084,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="18" thickBot="1">
+    <row r="261" spans="1:4" ht="17" thickBot="1">
       <c r="A261" s="19">
         <v>7636</v>
       </c>
@@ -5075,7 +5096,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="18" thickBot="1">
+    <row r="262" spans="1:4" ht="17" thickBot="1">
       <c r="A262" s="19">
         <v>7187</v>
       </c>
@@ -5087,7 +5108,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="18" thickBot="1">
+    <row r="263" spans="1:4" ht="17" thickBot="1">
       <c r="A263" s="19">
         <v>7188</v>
       </c>
@@ -5099,7 +5120,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="18" thickBot="1">
+    <row r="264" spans="1:4" ht="17" thickBot="1">
       <c r="A264" s="19">
         <v>7189</v>
       </c>
@@ -5111,7 +5132,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="18" thickBot="1">
+    <row r="265" spans="1:4" ht="17" thickBot="1">
       <c r="A265" s="19">
         <v>7190</v>
       </c>
@@ -5123,7 +5144,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="18" thickBot="1">
+    <row r="266" spans="1:4" ht="17" thickBot="1">
       <c r="A266" s="19">
         <v>7191</v>
       </c>
@@ -5135,7 +5156,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="18" thickBot="1">
+    <row r="267" spans="1:4" ht="17" thickBot="1">
       <c r="A267" s="19">
         <v>7192</v>
       </c>
@@ -5147,7 +5168,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="18" thickBot="1">
+    <row r="268" spans="1:4" ht="17" thickBot="1">
       <c r="A268" s="19">
         <v>7193</v>
       </c>
@@ -5159,7 +5180,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="18" thickBot="1">
+    <row r="269" spans="1:4" ht="17" thickBot="1">
       <c r="A269" s="19">
         <v>7635</v>
       </c>
@@ -5171,7 +5192,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="18" thickBot="1">
+    <row r="270" spans="1:4" ht="17" thickBot="1">
       <c r="A270" s="6">
         <v>5625</v>
       </c>
@@ -5183,7 +5204,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="18" thickBot="1">
+    <row r="271" spans="1:4" ht="17" thickBot="1">
       <c r="A271" s="6">
         <v>5626</v>
       </c>
@@ -5195,7 +5216,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="18" thickBot="1">
+    <row r="272" spans="1:4" ht="17" thickBot="1">
       <c r="A272" s="6">
         <v>5627</v>
       </c>
@@ -5207,7 +5228,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="18" thickBot="1">
+    <row r="273" spans="1:4" ht="17" thickBot="1">
       <c r="A273" s="6">
         <v>5628</v>
       </c>
@@ -5219,7 +5240,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="18" thickBot="1">
+    <row r="274" spans="1:4" ht="17" thickBot="1">
       <c r="A274" s="6">
         <v>8235</v>
       </c>
@@ -5231,7 +5252,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="18" thickBot="1">
+    <row r="275" spans="1:4" ht="17" thickBot="1">
       <c r="A275" s="6">
         <v>8236</v>
       </c>
@@ -5243,7 +5264,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="18" thickBot="1">
+    <row r="276" spans="1:4" ht="17" thickBot="1">
       <c r="A276" s="6">
         <v>8229</v>
       </c>
@@ -5255,7 +5276,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="18" thickBot="1">
+    <row r="277" spans="1:4" ht="17" thickBot="1">
       <c r="A277" s="6">
         <v>8230</v>
       </c>
@@ -5267,7 +5288,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="18" thickBot="1">
+    <row r="278" spans="1:4" ht="17" thickBot="1">
       <c r="A278" s="29">
         <v>8231</v>
       </c>
@@ -5279,7 +5300,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="18" thickBot="1">
+    <row r="279" spans="1:4" ht="17" thickBot="1">
       <c r="A279" s="6">
         <v>8232</v>
       </c>
@@ -5291,7 +5312,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="18" thickBot="1">
+    <row r="280" spans="1:4" ht="17" thickBot="1">
       <c r="A280" s="6">
         <v>8233</v>
       </c>
@@ -5303,7 +5324,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="18" thickBot="1">
+    <row r="281" spans="1:4" ht="17" thickBot="1">
       <c r="A281" s="6">
         <v>8234</v>
       </c>
@@ -5315,7 +5336,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="18" thickBot="1">
+    <row r="282" spans="1:4" ht="17" thickBot="1">
       <c r="A282" s="19">
         <v>7637</v>
       </c>
@@ -5327,7 +5348,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="18" thickBot="1">
+    <row r="283" spans="1:4" ht="17" thickBot="1">
       <c r="A283" s="19">
         <v>7638</v>
       </c>
@@ -5339,7 +5360,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="18" thickBot="1">
+    <row r="284" spans="1:4" ht="17" thickBot="1">
       <c r="A284" s="19">
         <v>7639</v>
       </c>
@@ -5351,7 +5372,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="18" thickBot="1">
+    <row r="285" spans="1:4" ht="17" thickBot="1">
       <c r="A285" s="19">
         <v>7640</v>
       </c>
@@ -5363,7 +5384,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="18" thickBot="1">
+    <row r="286" spans="1:4" ht="17" thickBot="1">
       <c r="A286" s="19">
         <v>7641</v>
       </c>
@@ -5375,7 +5396,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="18" thickBot="1">
+    <row r="287" spans="1:4" ht="17" thickBot="1">
       <c r="A287" s="19">
         <v>7642</v>
       </c>
@@ -5387,7 +5408,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="18" thickBot="1">
+    <row r="288" spans="1:4" ht="17" thickBot="1">
       <c r="A288" s="19">
         <v>7643</v>
       </c>
@@ -5399,7 +5420,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="18" thickBot="1">
+    <row r="289" spans="1:5" ht="17" thickBot="1">
       <c r="A289" s="19">
         <v>7644</v>
       </c>
@@ -5411,7 +5432,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="18" thickBot="1">
+    <row r="290" spans="1:5" ht="18" thickBot="1">
       <c r="A290" s="30">
         <v>1949</v>
       </c>
@@ -5423,7 +5444,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:5" ht="18" thickBot="1">
       <c r="A291" s="30">
         <v>7433</v>
       </c>
@@ -5434,6 +5455,69 @@
       <c r="D291" s="33">
         <v>226</v>
       </c>
+    </row>
+    <row r="292" spans="1:5" ht="18" thickBot="1">
+      <c r="A292" s="30">
+        <v>7452</v>
+      </c>
+      <c r="B292" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C292" s="32"/>
+      <c r="D292" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="18" thickBot="1">
+      <c r="A293" s="30">
+        <v>7296</v>
+      </c>
+      <c r="B293" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="C293" s="32"/>
+      <c r="D293" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="18" thickBot="1">
+      <c r="A294" s="30">
+        <v>7298</v>
+      </c>
+      <c r="B294" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="C294" s="32"/>
+      <c r="D294" s="35">
+        <v>226</v>
+      </c>
+      <c r="E294" s="36"/>
+    </row>
+    <row r="295" spans="1:5" ht="18" thickBot="1">
+      <c r="A295" s="30">
+        <v>6156</v>
+      </c>
+      <c r="B295" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="C295" s="32"/>
+      <c r="D295" s="35">
+        <v>226</v>
+      </c>
+      <c r="E295" s="36"/>
+    </row>
+    <row r="296" spans="1:5" ht="17">
+      <c r="A296" s="30">
+        <v>6157</v>
+      </c>
+      <c r="B296" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C296" s="32"/>
+      <c r="D296" s="35">
+        <v>226</v>
+      </c>
+      <c r="E296" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor code to generate orders dictionary and improve order processing efficiency
</commit_message>
<xml_diff>
--- a/sim/products.xlsx
+++ b/sim/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yossi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/black_disk/study/project_year_3/Picking/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B8C59B-C52F-4D21-A544-C92502F30CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304718A0-F165-554D-8B5D-CE7021CBE65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B8B0D30-750C-4C9D-85A7-B34DFC43DEF5}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="23260" windowHeight="14020" xr2:uid="{6B8B0D30-750C-4C9D-85A7-B34DFC43DEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Familys" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>item_id</t>
   </si>
@@ -935,6 +935,18 @@
   </si>
   <si>
     <t>זוג גופיות חצי שרוול איכותיות בגיר - מידה 3XL</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 1</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 2</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 3</t>
+  </si>
+  <si>
+    <t>בדיקה שקד 4</t>
   </si>
 </sst>
 </file>
@@ -945,7 +957,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -1589,7 +1601,24 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F56A6FD9-30DE-4534-9700-808734F282CD}" name="tbl_Familys" displayName="tbl_Familys" ref="A1:E291" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="A1:E291" xr:uid="{8781FA7B-3B84-43F7-B161-1EC7FB5AC567}"/>
+  <autoFilter ref="A1:E291" xr:uid="{8781FA7B-3B84-43F7-B161-1EC7FB5AC567}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="2074"/>
+        <filter val="7429"/>
+        <filter val="7430"/>
+        <filter val="7431"/>
+        <filter val="7432"/>
+        <filter val="7433"/>
+        <filter val="7435"/>
+        <filter val="7436"/>
+        <filter val="7437"/>
+        <filter val="7438"/>
+        <filter val="7439"/>
+        <filter val="7440"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D2">
     <sortCondition ref="D1:D2"/>
   </sortState>
@@ -1605,7 +1634,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1922,23 +1951,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A49E19-C7F0-4290-98E2-522667B31E5F}">
   <sheetPr codeName="גיליון8"/>
-  <dimension ref="A1:E291"/>
+  <dimension ref="A1:E295"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A185" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1">
+    <row r="1" spans="1:5" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1">
+    <row r="2" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A2" s="2">
         <v>7304</v>
       </c>
@@ -1967,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1">
+    <row r="3" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A3" s="6">
         <v>907</v>
       </c>
@@ -1979,7 +2008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1">
+    <row r="4" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A4" s="6">
         <v>5300</v>
       </c>
@@ -1991,7 +2020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1">
+    <row r="5" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A5" s="6">
         <v>831</v>
       </c>
@@ -2003,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" thickBot="1">
+    <row r="6" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A6" s="9">
         <v>1853</v>
       </c>
@@ -2015,7 +2044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" thickBot="1">
+    <row r="7" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A7" s="9">
         <v>5306</v>
       </c>
@@ -2027,7 +2056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" thickBot="1">
+    <row r="8" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A8" s="9">
         <v>1833</v>
       </c>
@@ -2039,7 +2068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1">
+    <row r="9" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A9" s="9">
         <v>1834</v>
       </c>
@@ -2051,7 +2080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" thickBot="1">
+    <row r="10" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A10" s="9">
         <v>6553</v>
       </c>
@@ -2063,7 +2092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" thickBot="1">
+    <row r="11" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A11" s="9">
         <v>1835</v>
       </c>
@@ -2075,7 +2104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" thickBot="1">
+    <row r="12" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A12" s="9">
         <v>1836</v>
       </c>
@@ -2087,7 +2116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" thickBot="1">
+    <row r="13" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A13" s="9">
         <v>1837</v>
       </c>
@@ -2099,7 +2128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" thickBot="1">
+    <row r="14" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A14" s="9">
         <v>1838</v>
       </c>
@@ -2111,7 +2140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" thickBot="1">
+    <row r="15" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A15" s="9">
         <v>1839</v>
       </c>
@@ -2123,7 +2152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" thickBot="1">
+    <row r="16" spans="1:5" ht="17" hidden="1" thickBot="1">
       <c r="A16" s="9">
         <v>1840</v>
       </c>
@@ -2135,7 +2164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1">
+    <row r="17" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A17" s="9">
         <v>1841</v>
       </c>
@@ -2147,7 +2176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" thickBot="1">
+    <row r="18" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A18" s="9">
         <v>1842</v>
       </c>
@@ -2159,7 +2188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1">
+    <row r="19" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A19" s="9">
         <v>1843</v>
       </c>
@@ -2171,7 +2200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1">
+    <row r="20" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A20" s="9">
         <v>1844</v>
       </c>
@@ -2183,7 +2212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1">
+    <row r="21" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A21" s="9">
         <v>1845</v>
       </c>
@@ -2195,7 +2224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1">
+    <row r="22" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A22" s="9">
         <v>1846</v>
       </c>
@@ -2207,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1">
+    <row r="23" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A23" s="9">
         <v>1847</v>
       </c>
@@ -2219,7 +2248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" thickBot="1">
+    <row r="24" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A24" s="9">
         <v>1848</v>
       </c>
@@ -2231,7 +2260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1">
+    <row r="25" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A25" s="9">
         <v>1849</v>
       </c>
@@ -2243,7 +2272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1">
+    <row r="26" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A26" s="9">
         <v>1850</v>
       </c>
@@ -2255,7 +2284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1">
+    <row r="27" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A27" s="9">
         <v>1851</v>
       </c>
@@ -2267,7 +2296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1">
+    <row r="28" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A28" s="9">
         <v>1852</v>
       </c>
@@ -2279,7 +2308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1">
+    <row r="29" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A29" s="9">
         <v>5378</v>
       </c>
@@ -2291,7 +2320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" thickBot="1">
+    <row r="30" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A30" s="9">
         <v>5379</v>
       </c>
@@ -2303,7 +2332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" thickBot="1">
+    <row r="31" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A31" s="9">
         <v>6551</v>
       </c>
@@ -2315,7 +2344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1">
+    <row r="32" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A32" s="9">
         <v>6552</v>
       </c>
@@ -2327,7 +2356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" thickBot="1">
+    <row r="33" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A33" s="9">
         <v>6055</v>
       </c>
@@ -2339,7 +2368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" thickBot="1">
+    <row r="34" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A34" s="9">
         <v>6056</v>
       </c>
@@ -2351,7 +2380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" thickBot="1">
+    <row r="35" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A35" s="9">
         <v>6057</v>
       </c>
@@ -2363,7 +2392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" thickBot="1">
+    <row r="36" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A36" s="9">
         <v>6058</v>
       </c>
@@ -2375,7 +2404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" thickBot="1">
+    <row r="37" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A37" s="9">
         <v>6059</v>
       </c>
@@ -2387,7 +2416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1">
+    <row r="38" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A38" s="9">
         <v>6060</v>
       </c>
@@ -2399,7 +2428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" thickBot="1">
+    <row r="39" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A39" s="9">
         <v>6061</v>
       </c>
@@ -2411,7 +2440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" thickBot="1">
+    <row r="40" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A40" s="9">
         <v>6062</v>
       </c>
@@ -2423,7 +2452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" thickBot="1">
+    <row r="41" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A41" s="9">
         <v>6063</v>
       </c>
@@ -2435,7 +2464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" thickBot="1">
+    <row r="42" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A42" s="9">
         <v>6064</v>
       </c>
@@ -2447,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" thickBot="1">
+    <row r="43" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A43" s="9">
         <v>6065</v>
       </c>
@@ -2459,7 +2488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18" thickBot="1">
+    <row r="44" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A44" s="9">
         <v>6066</v>
       </c>
@@ -2471,7 +2500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18" thickBot="1">
+    <row r="45" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A45" s="9">
         <v>6067</v>
       </c>
@@ -2483,7 +2512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18" thickBot="1">
+    <row r="46" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A46" s="9">
         <v>6068</v>
       </c>
@@ -2495,7 +2524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18" thickBot="1">
+    <row r="47" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A47" s="9">
         <v>6069</v>
       </c>
@@ -2507,7 +2536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18" thickBot="1">
+    <row r="48" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A48" s="9">
         <v>6070</v>
       </c>
@@ -2519,7 +2548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18" thickBot="1">
+    <row r="49" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A49" s="6">
         <v>6071</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18" thickBot="1">
+    <row r="50" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A50" s="6">
         <v>2499</v>
       </c>
@@ -2543,7 +2572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18" thickBot="1">
+    <row r="51" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A51" s="6">
         <v>7847</v>
       </c>
@@ -2555,7 +2584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18" thickBot="1">
+    <row r="52" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A52" s="6">
         <v>7848</v>
       </c>
@@ -2567,7 +2596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18" thickBot="1">
+    <row r="53" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A53" s="6">
         <v>7849</v>
       </c>
@@ -2579,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="18" thickBot="1">
+    <row r="54" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A54" s="6">
         <v>7850</v>
       </c>
@@ -2591,7 +2620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18" thickBot="1">
+    <row r="55" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A55" s="6">
         <v>7851</v>
       </c>
@@ -2603,7 +2632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="18" thickBot="1">
+    <row r="56" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A56" s="6">
         <v>7852</v>
       </c>
@@ -2615,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="18" thickBot="1">
+    <row r="57" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A57" s="6">
         <v>7853</v>
       </c>
@@ -2627,7 +2656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" thickBot="1">
+    <row r="58" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A58" s="6">
         <v>7854</v>
       </c>
@@ -2639,7 +2668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="18" thickBot="1">
+    <row r="59" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A59" s="6">
         <v>7855</v>
       </c>
@@ -2651,7 +2680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="18" thickBot="1">
+    <row r="60" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A60" s="6">
         <v>7856</v>
       </c>
@@ -2663,7 +2692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="18" thickBot="1">
+    <row r="61" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A61" s="6">
         <v>7857</v>
       </c>
@@ -2675,7 +2704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18" thickBot="1">
+    <row r="62" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A62" s="6">
         <v>7858</v>
       </c>
@@ -2687,7 +2716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18" thickBot="1">
+    <row r="63" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A63" s="6">
         <v>7859</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="18" thickBot="1">
+    <row r="64" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A64" s="6">
         <v>7860</v>
       </c>
@@ -2711,7 +2740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18" thickBot="1">
+    <row r="65" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A65" s="6">
         <v>7861</v>
       </c>
@@ -2723,7 +2752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="18" thickBot="1">
+    <row r="66" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A66" s="6">
         <v>7862</v>
       </c>
@@ -2735,7 +2764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="18" thickBot="1">
+    <row r="67" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A67" s="6">
         <v>7863</v>
       </c>
@@ -2747,7 +2776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="18" thickBot="1">
+    <row r="68" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A68" s="6">
         <v>7864</v>
       </c>
@@ -2759,7 +2788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="18" thickBot="1">
+    <row r="69" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A69" s="6">
         <v>7865</v>
       </c>
@@ -2771,7 +2800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="18" thickBot="1">
+    <row r="70" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A70" s="6">
         <v>2498</v>
       </c>
@@ -2783,7 +2812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="18" thickBot="1">
+    <row r="71" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A71" s="6">
         <v>5304</v>
       </c>
@@ -2795,7 +2824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="18" thickBot="1">
+    <row r="72" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A72" s="6">
         <v>2030</v>
       </c>
@@ -2807,7 +2836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="18" thickBot="1">
+    <row r="73" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A73" s="6">
         <v>5837</v>
       </c>
@@ -2819,7 +2848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="18" thickBot="1">
+    <row r="74" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A74" s="6">
         <v>5617</v>
       </c>
@@ -2831,7 +2860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="18" thickBot="1">
+    <row r="75" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A75" s="6">
         <v>5384</v>
       </c>
@@ -2843,7 +2872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="18" thickBot="1">
+    <row r="76" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A76" s="6">
         <v>5753</v>
       </c>
@@ -2855,7 +2884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="18" thickBot="1">
+    <row r="77" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A77" s="6">
         <v>6164</v>
       </c>
@@ -2867,7 +2896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="18" thickBot="1">
+    <row r="78" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A78" s="6">
         <v>5383</v>
       </c>
@@ -2879,7 +2908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18" thickBot="1">
+    <row r="79" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A79" s="6">
         <v>5754</v>
       </c>
@@ -2891,7 +2920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="18" thickBot="1">
+    <row r="80" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A80" s="13">
         <v>2380</v>
       </c>
@@ -2903,7 +2932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="18" thickBot="1">
+    <row r="81" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A81" s="13">
         <v>2381</v>
       </c>
@@ -2915,7 +2944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18" thickBot="1">
+    <row r="82" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A82" s="13">
         <v>2382</v>
       </c>
@@ -2927,7 +2956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="18" thickBot="1">
+    <row r="83" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A83" s="13">
         <v>2383</v>
       </c>
@@ -2939,7 +2968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="18" thickBot="1">
+    <row r="84" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A84" s="9">
         <v>5609</v>
       </c>
@@ -2951,7 +2980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18" thickBot="1">
+    <row r="85" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A85" s="9">
         <v>5610</v>
       </c>
@@ -2963,7 +2992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="18" thickBot="1">
+    <row r="86" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A86" s="13">
         <v>5611</v>
       </c>
@@ -2975,7 +3004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="18" thickBot="1">
+    <row r="87" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A87" s="13">
         <v>5612</v>
       </c>
@@ -2987,7 +3016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="18" thickBot="1">
+    <row r="88" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A88" s="13">
         <v>5613</v>
       </c>
@@ -2999,7 +3028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18" thickBot="1">
+    <row r="89" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A89" s="13">
         <v>5614</v>
       </c>
@@ -3011,7 +3040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="18" thickBot="1">
+    <row r="90" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A90" s="13">
         <v>5615</v>
       </c>
@@ -3023,7 +3052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="18" thickBot="1">
+    <row r="91" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A91" s="13">
         <v>5616</v>
       </c>
@@ -3035,7 +3064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="18" thickBot="1">
+    <row r="92" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A92" s="6">
         <v>7313</v>
       </c>
@@ -3047,7 +3076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="18" thickBot="1">
+    <row r="93" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A93" s="6">
         <v>7312</v>
       </c>
@@ -3059,7 +3088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="18" thickBot="1">
+    <row r="94" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A94" s="6">
         <v>7314</v>
       </c>
@@ -3071,7 +3100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="18" thickBot="1">
+    <row r="95" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A95" s="6">
         <v>7315</v>
       </c>
@@ -3083,7 +3112,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="18" thickBot="1">
+    <row r="96" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A96" s="13">
         <v>7976</v>
       </c>
@@ -3095,7 +3124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="18" thickBot="1">
+    <row r="97" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A97" s="13">
         <v>7977</v>
       </c>
@@ -3107,7 +3136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="18" thickBot="1">
+    <row r="98" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A98" s="13">
         <v>7978</v>
       </c>
@@ -3119,7 +3148,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="18" thickBot="1">
+    <row r="99" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A99" s="13">
         <v>7979</v>
       </c>
@@ -3131,7 +3160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="18" thickBot="1">
+    <row r="100" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A100" s="13">
         <v>2234</v>
       </c>
@@ -3143,7 +3172,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="18" thickBot="1">
+    <row r="101" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A101" s="13">
         <v>2235</v>
       </c>
@@ -3155,7 +3184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="18" thickBot="1">
+    <row r="102" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A102" s="13">
         <v>2236</v>
       </c>
@@ -3167,7 +3196,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="18" thickBot="1">
+    <row r="103" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A103" s="13">
         <v>2237</v>
       </c>
@@ -3179,7 +3208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="18" thickBot="1">
+    <row r="104" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A104" s="13">
         <v>2238</v>
       </c>
@@ -3191,7 +3220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="18" thickBot="1">
+    <row r="105" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A105" s="13">
         <v>6406</v>
       </c>
@@ -3203,7 +3232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="18" thickBot="1">
+    <row r="106" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A106" s="6">
         <v>7980</v>
       </c>
@@ -3215,7 +3244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="18" thickBot="1">
+    <row r="107" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A107" s="13">
         <v>7885</v>
       </c>
@@ -3227,7 +3256,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="18" thickBot="1">
+    <row r="108" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A108" s="13">
         <v>7886</v>
       </c>
@@ -3239,7 +3268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="18" thickBot="1">
+    <row r="109" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A109" s="13">
         <v>7887</v>
       </c>
@@ -3251,7 +3280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="18" thickBot="1">
+    <row r="110" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A110" s="13">
         <v>7888</v>
       </c>
@@ -3263,7 +3292,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="18" thickBot="1">
+    <row r="111" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A111" s="13">
         <v>7889</v>
       </c>
@@ -3275,7 +3304,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="18" thickBot="1">
+    <row r="112" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A112" s="13">
         <v>7890</v>
       </c>
@@ -3287,7 +3316,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="18" thickBot="1">
+    <row r="113" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A113" s="6">
         <v>5978</v>
       </c>
@@ -3299,7 +3328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="18" thickBot="1">
+    <row r="114" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A114" s="6">
         <v>5979</v>
       </c>
@@ -3311,7 +3340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="18" thickBot="1">
+    <row r="115" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A115" s="6">
         <v>5980</v>
       </c>
@@ -3323,7 +3352,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="18" thickBot="1">
+    <row r="116" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A116" s="6">
         <v>5981</v>
       </c>
@@ -3335,7 +3364,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="18" thickBot="1">
+    <row r="117" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A117" s="6">
         <v>5982</v>
       </c>
@@ -3347,7 +3376,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="18" thickBot="1">
+    <row r="118" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A118" s="6">
         <v>5983</v>
       </c>
@@ -3359,7 +3388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="18" thickBot="1">
+    <row r="119" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A119" s="13">
         <v>7770</v>
       </c>
@@ -3371,7 +3400,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="18" thickBot="1">
+    <row r="120" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A120" s="13">
         <v>7772</v>
       </c>
@@ -3383,7 +3412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="18" thickBot="1">
+    <row r="121" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A121" s="13">
         <v>7773</v>
       </c>
@@ -3395,7 +3424,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="18" thickBot="1">
+    <row r="122" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A122" s="6">
         <v>7964</v>
       </c>
@@ -3407,7 +3436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="18" thickBot="1">
+    <row r="123" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A123" s="6">
         <v>5145</v>
       </c>
@@ -3419,7 +3448,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="18" thickBot="1">
+    <row r="124" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A124" s="6">
         <v>5141</v>
       </c>
@@ -3431,7 +3460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="18" thickBot="1">
+    <row r="125" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A125" s="6">
         <v>5142</v>
       </c>
@@ -3443,7 +3472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="18" thickBot="1">
+    <row r="126" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A126" s="6">
         <v>5143</v>
       </c>
@@ -3455,7 +3484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="18" thickBot="1">
+    <row r="127" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A127" s="6">
         <v>5144</v>
       </c>
@@ -3467,7 +3496,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="18" thickBot="1">
+    <row r="128" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A128" s="6">
         <v>5836</v>
       </c>
@@ -3479,7 +3508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="18" thickBot="1">
+    <row r="129" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A129" s="6">
         <v>8156</v>
       </c>
@@ -3491,7 +3520,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="18" thickBot="1">
+    <row r="130" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A130" s="6">
         <v>8157</v>
       </c>
@@ -3503,7 +3532,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="18" thickBot="1">
+    <row r="131" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A131" s="9">
         <v>2449</v>
       </c>
@@ -3515,7 +3544,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="18" thickBot="1">
+    <row r="132" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A132" s="6">
         <v>8159</v>
       </c>
@@ -3527,7 +3556,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="18" thickBot="1">
+    <row r="133" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A133" s="6">
         <v>8160</v>
       </c>
@@ -3539,7 +3568,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="18" thickBot="1">
+    <row r="134" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A134" s="6">
         <v>8161</v>
       </c>
@@ -3551,7 +3580,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="18" thickBot="1">
+    <row r="135" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A135" s="9">
         <v>8099</v>
       </c>
@@ -3563,7 +3592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="18" thickBot="1">
+    <row r="136" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A136" s="9">
         <v>8083</v>
       </c>
@@ -3575,7 +3604,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="18" thickBot="1">
+    <row r="137" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A137" s="9">
         <v>8141</v>
       </c>
@@ -3587,7 +3616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="18" thickBot="1">
+    <row r="138" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A138" s="9">
         <v>8139</v>
       </c>
@@ -3599,7 +3628,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="18" thickBot="1">
+    <row r="139" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A139" s="9">
         <v>8142</v>
       </c>
@@ -3611,7 +3640,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="18" thickBot="1">
+    <row r="140" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A140" s="18">
         <v>8081</v>
       </c>
@@ -3623,7 +3652,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="18" thickBot="1">
+    <row r="141" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A141" s="18">
         <v>8082</v>
       </c>
@@ -3635,7 +3664,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="18" thickBot="1">
+    <row r="142" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A142" s="18">
         <v>8084</v>
       </c>
@@ -3647,7 +3676,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="18" thickBot="1">
+    <row r="143" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A143" s="5">
         <v>8140</v>
       </c>
@@ -3659,7 +3688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="18" thickBot="1">
+    <row r="144" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A144" s="5">
         <v>8138</v>
       </c>
@@ -3671,7 +3700,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="18" thickBot="1">
+    <row r="145" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A145" s="5">
         <v>8080</v>
       </c>
@@ -3683,7 +3712,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="18" thickBot="1">
+    <row r="146" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A146" s="5">
         <v>8137</v>
       </c>
@@ -3695,7 +3724,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="18" thickBot="1">
+    <row r="147" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A147" s="5">
         <v>8079</v>
       </c>
@@ -3707,7 +3736,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="18" thickBot="1">
+    <row r="148" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A148" s="5">
         <v>7305</v>
       </c>
@@ -3719,7 +3748,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="18" thickBot="1">
+    <row r="149" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A149" s="5">
         <v>7307</v>
       </c>
@@ -3731,7 +3760,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="18" thickBot="1">
+    <row r="150" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A150" s="5">
         <v>7634</v>
       </c>
@@ -3743,7 +3772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="18" thickBot="1">
+    <row r="151" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A151" s="5">
         <v>7765</v>
       </c>
@@ -3755,7 +3784,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="18" thickBot="1">
+    <row r="152" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A152" s="5">
         <v>7884</v>
       </c>
@@ -3767,7 +3796,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="18" thickBot="1">
+    <row r="153" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A153" s="19">
         <v>5835</v>
       </c>
@@ -3779,7 +3808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="18" thickBot="1">
+    <row r="154" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A154" s="19">
         <v>1948</v>
       </c>
@@ -3791,7 +3820,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="18" thickBot="1">
+    <row r="155" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A155" s="19">
         <v>7755</v>
       </c>
@@ -3803,7 +3832,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="18" thickBot="1">
+    <row r="156" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A156" s="22">
         <v>1942</v>
       </c>
@@ -3815,7 +3844,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="18" thickBot="1">
+    <row r="157" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A157" s="22">
         <v>1943</v>
       </c>
@@ -3827,7 +3856,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="18" thickBot="1">
+    <row r="158" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A158" s="22">
         <v>1944</v>
       </c>
@@ -3839,7 +3868,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="18" thickBot="1">
+    <row r="159" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A159" s="22">
         <v>2384</v>
       </c>
@@ -3851,7 +3880,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="18" thickBot="1">
+    <row r="160" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A160" s="22">
         <v>2385</v>
       </c>
@@ -3863,7 +3892,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="18" thickBot="1">
+    <row r="161" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A161" s="22">
         <v>2460</v>
       </c>
@@ -3875,7 +3904,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="18" thickBot="1">
+    <row r="162" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A162" s="22">
         <v>5020</v>
       </c>
@@ -3887,7 +3916,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="18" thickBot="1">
+    <row r="163" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A163" s="22">
         <v>5377</v>
       </c>
@@ -3899,7 +3928,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="18" thickBot="1">
+    <row r="164" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A164" s="22">
         <v>2075</v>
       </c>
@@ -3911,7 +3940,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="18" thickBot="1">
+    <row r="165" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A165" s="22">
         <v>1928</v>
       </c>
@@ -3923,7 +3952,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="18" thickBot="1">
+    <row r="166" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A166" s="22">
         <v>1929</v>
       </c>
@@ -3935,7 +3964,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="18" thickBot="1">
+    <row r="167" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A167" s="22">
         <v>1930</v>
       </c>
@@ -3947,7 +3976,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="18" thickBot="1">
+    <row r="168" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A168" s="22">
         <v>1933</v>
       </c>
@@ -3959,7 +3988,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="18" thickBot="1">
+    <row r="169" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A169" s="22">
         <v>1934</v>
       </c>
@@ -3971,7 +4000,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="18" thickBot="1">
+    <row r="170" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A170" s="22">
         <v>1931</v>
       </c>
@@ -3983,7 +4012,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="18" thickBot="1">
+    <row r="171" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A171" s="22">
         <v>1932</v>
       </c>
@@ -3995,7 +4024,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="18" thickBot="1">
+    <row r="172" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A172" s="22">
         <v>6407</v>
       </c>
@@ -4007,7 +4036,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="18" thickBot="1">
+    <row r="173" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A173" s="22">
         <v>784</v>
       </c>
@@ -4019,7 +4048,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="18" thickBot="1">
+    <row r="174" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A174" s="22">
         <v>1953</v>
       </c>
@@ -4031,7 +4060,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="18" thickBot="1">
+    <row r="175" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A175" s="22">
         <v>1950</v>
       </c>
@@ -4043,7 +4072,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="18" thickBot="1">
+    <row r="176" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A176" s="22">
         <v>1951</v>
       </c>
@@ -4055,7 +4084,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="18" thickBot="1">
+    <row r="177" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A177" s="22">
         <v>1952</v>
       </c>
@@ -4067,7 +4096,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="18" thickBot="1">
+    <row r="178" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A178" s="23">
         <v>2031</v>
       </c>
@@ -4079,7 +4108,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="18" thickBot="1">
+    <row r="179" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A179" s="9">
         <v>2461</v>
       </c>
@@ -4091,7 +4120,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="18" thickBot="1">
+    <row r="180" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A180" s="23">
         <v>6517</v>
       </c>
@@ -4103,7 +4132,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="18" thickBot="1">
+    <row r="181" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A181" s="22">
         <v>6705</v>
       </c>
@@ -4115,7 +4144,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="18" thickBot="1">
+    <row r="182" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A182" s="26">
         <v>2032</v>
       </c>
@@ -4127,7 +4156,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="18" thickBot="1">
+    <row r="183" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A183" s="26">
         <v>2033</v>
       </c>
@@ -4139,7 +4168,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="18" thickBot="1">
+    <row r="184" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A184" s="26">
         <v>750</v>
       </c>
@@ -4151,7 +4180,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="18" thickBot="1">
+    <row r="185" spans="1:4" ht="17" thickBot="1">
       <c r="A185" s="26">
         <v>2074</v>
       </c>
@@ -4163,7 +4192,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="18" thickBot="1">
+    <row r="186" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A186" s="26">
         <v>1937</v>
       </c>
@@ -4175,7 +4204,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="18" thickBot="1">
+    <row r="187" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A187" s="26">
         <v>1935</v>
       </c>
@@ -4187,7 +4216,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="18" thickBot="1">
+    <row r="188" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A188" s="26">
         <v>1936</v>
       </c>
@@ -4199,7 +4228,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="18" thickBot="1">
+    <row r="189" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A189" s="26">
         <v>1938</v>
       </c>
@@ -4211,7 +4240,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="18" thickBot="1">
+    <row r="190" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A190" s="26">
         <v>1939</v>
       </c>
@@ -4223,7 +4252,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="18" thickBot="1">
+    <row r="191" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A191" s="22">
         <v>1940</v>
       </c>
@@ -4235,7 +4264,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="18" thickBot="1">
+    <row r="192" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A192" s="22">
         <v>1941</v>
       </c>
@@ -4247,7 +4276,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="18" thickBot="1">
+    <row r="193" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A193" s="22">
         <v>6536</v>
       </c>
@@ -4259,7 +4288,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="18" thickBot="1">
+    <row r="194" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A194" s="22">
         <v>5149</v>
       </c>
@@ -4271,7 +4300,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="18" thickBot="1">
+    <row r="195" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A195" s="22">
         <v>5150</v>
       </c>
@@ -4283,7 +4312,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="18" thickBot="1">
+    <row r="196" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A196" s="22">
         <v>5151</v>
       </c>
@@ -4295,7 +4324,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="18" thickBot="1">
+    <row r="197" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A197" s="22">
         <v>5152</v>
       </c>
@@ -4307,7 +4336,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="18" thickBot="1">
+    <row r="198" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A198" s="22">
         <v>5153</v>
       </c>
@@ -4319,7 +4348,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="18" thickBot="1">
+    <row r="199" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A199" s="22">
         <v>5376</v>
       </c>
@@ -4331,7 +4360,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="18" thickBot="1">
+    <row r="200" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A200" s="19">
         <v>5310</v>
       </c>
@@ -4343,7 +4372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="18" thickBot="1">
+    <row r="201" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A201" s="19">
         <v>7015</v>
       </c>
@@ -4355,7 +4384,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="18" thickBot="1">
+    <row r="202" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A202" s="25">
         <v>7016</v>
       </c>
@@ -4367,7 +4396,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="18" thickBot="1">
+    <row r="203" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A203" s="19">
         <v>7017</v>
       </c>
@@ -4379,7 +4408,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="18" thickBot="1">
+    <row r="204" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A204" s="19">
         <v>7018</v>
       </c>
@@ -4391,7 +4420,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="18" thickBot="1">
+    <row r="205" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A205" s="19">
         <v>7019</v>
       </c>
@@ -4403,7 +4432,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="18" thickBot="1">
+    <row r="206" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A206" s="19">
         <v>7020</v>
       </c>
@@ -4415,7 +4444,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="18" thickBot="1">
+    <row r="207" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A207" s="19">
         <v>7021</v>
       </c>
@@ -4427,7 +4456,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="18" thickBot="1">
+    <row r="208" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A208" s="19">
         <v>1922</v>
       </c>
@@ -4439,7 +4468,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="18" thickBot="1">
+    <row r="209" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A209" s="19">
         <v>1923</v>
       </c>
@@ -4451,7 +4480,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="18" thickBot="1">
+    <row r="210" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A210" s="19">
         <v>1924</v>
       </c>
@@ -4463,7 +4492,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="18" thickBot="1">
+    <row r="211" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A211" s="19">
         <v>1925</v>
       </c>
@@ -4475,7 +4504,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="18" thickBot="1">
+    <row r="212" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A212" s="19">
         <v>1926</v>
       </c>
@@ -4487,7 +4516,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="18" thickBot="1">
+    <row r="213" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A213" s="19">
         <v>1927</v>
       </c>
@@ -4499,7 +4528,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="18" thickBot="1">
+    <row r="214" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A214" s="19">
         <v>2091</v>
       </c>
@@ -4511,7 +4540,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="18" thickBot="1">
+    <row r="215" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A215" s="19">
         <v>2077</v>
       </c>
@@ -4523,7 +4552,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="18" thickBot="1">
+    <row r="216" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A216" s="19">
         <v>2078</v>
       </c>
@@ -4535,7 +4564,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="18" thickBot="1">
+    <row r="217" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A217" s="19">
         <v>2079</v>
       </c>
@@ -4547,7 +4576,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="18" thickBot="1">
+    <row r="218" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A218" s="19">
         <v>2080</v>
       </c>
@@ -4559,7 +4588,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="18" thickBot="1">
+    <row r="219" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A219" s="19">
         <v>2081</v>
       </c>
@@ -4571,7 +4600,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="18" thickBot="1">
+    <row r="220" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A220" s="20">
         <v>7299</v>
       </c>
@@ -4583,7 +4612,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="18" thickBot="1">
+    <row r="221" spans="1:4" ht="17" thickBot="1">
       <c r="A221" s="19">
         <v>7429</v>
       </c>
@@ -4595,7 +4624,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="18" thickBot="1">
+    <row r="222" spans="1:4" ht="17" thickBot="1">
       <c r="A222" s="19">
         <v>7430</v>
       </c>
@@ -4607,7 +4636,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="18" thickBot="1">
+    <row r="223" spans="1:4" ht="17" thickBot="1">
       <c r="A223" s="19">
         <v>7431</v>
       </c>
@@ -4619,7 +4648,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="18" thickBot="1">
+    <row r="224" spans="1:4" ht="17" thickBot="1">
       <c r="A224" s="19">
         <v>7432</v>
       </c>
@@ -4631,7 +4660,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="18" thickBot="1">
+    <row r="225" spans="1:4" ht="17" thickBot="1">
       <c r="A225" s="19">
         <v>7435</v>
       </c>
@@ -4643,7 +4672,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="18" thickBot="1">
+    <row r="226" spans="1:4" ht="17" thickBot="1">
       <c r="A226" s="19">
         <v>7436</v>
       </c>
@@ -4655,7 +4684,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="18" thickBot="1">
+    <row r="227" spans="1:4" ht="17" thickBot="1">
       <c r="A227" s="19">
         <v>7437</v>
       </c>
@@ -4667,7 +4696,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="18" thickBot="1">
+    <row r="228" spans="1:4" ht="17" thickBot="1">
       <c r="A228" s="19">
         <v>7438</v>
       </c>
@@ -4679,7 +4708,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="18" thickBot="1">
+    <row r="229" spans="1:4" ht="17" thickBot="1">
       <c r="A229" s="19">
         <v>7439</v>
       </c>
@@ -4691,7 +4720,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="18" thickBot="1">
+    <row r="230" spans="1:4" ht="17" thickBot="1">
       <c r="A230" s="19">
         <v>7440</v>
       </c>
@@ -4703,7 +4732,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="18" thickBot="1">
+    <row r="231" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A231" s="19">
         <v>8312</v>
       </c>
@@ -4715,7 +4744,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="18" thickBot="1">
+    <row r="232" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A232" s="19">
         <v>8313</v>
       </c>
@@ -4727,7 +4756,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="18" thickBot="1">
+    <row r="233" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A233" s="19">
         <v>8314</v>
       </c>
@@ -4739,7 +4768,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="18" thickBot="1">
+    <row r="234" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A234" s="19">
         <v>2402</v>
       </c>
@@ -4751,7 +4780,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="18" thickBot="1">
+    <row r="235" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A235" s="19">
         <v>2403</v>
       </c>
@@ -4763,7 +4792,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="18" thickBot="1">
+    <row r="236" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A236" s="19">
         <v>2404</v>
       </c>
@@ -4775,7 +4804,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="18" thickBot="1">
+    <row r="237" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A237" s="19">
         <v>2405</v>
       </c>
@@ -4787,7 +4816,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="18" thickBot="1">
+    <row r="238" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A238" s="19">
         <v>5302</v>
       </c>
@@ -4799,7 +4828,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="18" thickBot="1">
+    <row r="239" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A239" s="19">
         <v>7303</v>
       </c>
@@ -4811,7 +4840,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="18" thickBot="1">
+    <row r="240" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A240" s="13">
         <v>2199</v>
       </c>
@@ -4823,7 +4852,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="18" thickBot="1">
+    <row r="241" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A241" s="13">
         <v>2200</v>
       </c>
@@ -4835,7 +4864,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="18" thickBot="1">
+    <row r="242" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A242" s="13">
         <v>2201</v>
       </c>
@@ -4847,7 +4876,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="18" thickBot="1">
+    <row r="243" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A243" s="13">
         <v>2202</v>
       </c>
@@ -4859,7 +4888,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="18" thickBot="1">
+    <row r="244" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A244" s="13">
         <v>2203</v>
       </c>
@@ -4871,7 +4900,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="18" thickBot="1">
+    <row r="245" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A245" s="13">
         <v>5162</v>
       </c>
@@ -4883,7 +4912,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="18" thickBot="1">
+    <row r="246" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A246" s="19">
         <v>7175</v>
       </c>
@@ -4895,7 +4924,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="18" thickBot="1">
+    <row r="247" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A247" s="19">
         <v>7211</v>
       </c>
@@ -4907,7 +4936,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="18" thickBot="1">
+    <row r="248" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A248" s="19">
         <v>7604</v>
       </c>
@@ -4919,7 +4948,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="18" thickBot="1">
+    <row r="249" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A249" s="19">
         <v>7564</v>
       </c>
@@ -4931,7 +4960,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="18" thickBot="1">
+    <row r="250" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A250" s="19">
         <v>7565</v>
       </c>
@@ -4943,7 +4972,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="18" thickBot="1">
+    <row r="251" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A251" s="19">
         <v>7566</v>
       </c>
@@ -4955,7 +4984,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="18" thickBot="1">
+    <row r="252" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A252" s="19">
         <v>7290</v>
       </c>
@@ -4967,7 +4996,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="18" thickBot="1">
+    <row r="253" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A253" s="19">
         <v>7295</v>
       </c>
@@ -4979,7 +5008,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="18" thickBot="1">
+    <row r="254" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A254" s="19">
         <v>7180</v>
       </c>
@@ -4991,7 +5020,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="18" thickBot="1">
+    <row r="255" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A255" s="19">
         <v>7181</v>
       </c>
@@ -5003,7 +5032,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="18" thickBot="1">
+    <row r="256" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A256" s="19">
         <v>7182</v>
       </c>
@@ -5015,7 +5044,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="18" thickBot="1">
+    <row r="257" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A257" s="19">
         <v>7183</v>
       </c>
@@ -5027,7 +5056,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="18" thickBot="1">
+    <row r="258" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A258" s="19">
         <v>7184</v>
       </c>
@@ -5039,7 +5068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="18" thickBot="1">
+    <row r="259" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A259" s="19">
         <v>7185</v>
       </c>
@@ -5051,7 +5080,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="18" thickBot="1">
+    <row r="260" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A260" s="19">
         <v>7186</v>
       </c>
@@ -5063,7 +5092,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="18" thickBot="1">
+    <row r="261" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A261" s="19">
         <v>7636</v>
       </c>
@@ -5075,7 +5104,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="18" thickBot="1">
+    <row r="262" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A262" s="19">
         <v>7187</v>
       </c>
@@ -5087,7 +5116,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="18" thickBot="1">
+    <row r="263" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A263" s="19">
         <v>7188</v>
       </c>
@@ -5099,7 +5128,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="18" thickBot="1">
+    <row r="264" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A264" s="19">
         <v>7189</v>
       </c>
@@ -5111,7 +5140,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="18" thickBot="1">
+    <row r="265" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A265" s="19">
         <v>7190</v>
       </c>
@@ -5123,7 +5152,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="18" thickBot="1">
+    <row r="266" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A266" s="19">
         <v>7191</v>
       </c>
@@ -5135,7 +5164,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="18" thickBot="1">
+    <row r="267" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A267" s="19">
         <v>7192</v>
       </c>
@@ -5147,7 +5176,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="18" thickBot="1">
+    <row r="268" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A268" s="19">
         <v>7193</v>
       </c>
@@ -5159,7 +5188,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="18" thickBot="1">
+    <row r="269" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A269" s="19">
         <v>7635</v>
       </c>
@@ -5171,7 +5200,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="18" thickBot="1">
+    <row r="270" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A270" s="6">
         <v>5625</v>
       </c>
@@ -5183,7 +5212,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="18" thickBot="1">
+    <row r="271" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A271" s="6">
         <v>5626</v>
       </c>
@@ -5195,7 +5224,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="18" thickBot="1">
+    <row r="272" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A272" s="6">
         <v>5627</v>
       </c>
@@ -5207,7 +5236,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="18" thickBot="1">
+    <row r="273" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A273" s="6">
         <v>5628</v>
       </c>
@@ -5219,7 +5248,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="18" thickBot="1">
+    <row r="274" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A274" s="6">
         <v>8235</v>
       </c>
@@ -5231,7 +5260,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="18" thickBot="1">
+    <row r="275" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A275" s="6">
         <v>8236</v>
       </c>
@@ -5243,7 +5272,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="18" thickBot="1">
+    <row r="276" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A276" s="6">
         <v>8229</v>
       </c>
@@ -5255,7 +5284,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="18" thickBot="1">
+    <row r="277" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A277" s="6">
         <v>8230</v>
       </c>
@@ -5267,7 +5296,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="18" thickBot="1">
+    <row r="278" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A278" s="29">
         <v>8231</v>
       </c>
@@ -5279,7 +5308,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="18" thickBot="1">
+    <row r="279" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A279" s="6">
         <v>8232</v>
       </c>
@@ -5291,7 +5320,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="18" thickBot="1">
+    <row r="280" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A280" s="6">
         <v>8233</v>
       </c>
@@ -5303,7 +5332,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="18" thickBot="1">
+    <row r="281" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A281" s="6">
         <v>8234</v>
       </c>
@@ -5315,7 +5344,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="18" thickBot="1">
+    <row r="282" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A282" s="19">
         <v>7637</v>
       </c>
@@ -5327,7 +5356,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="18" thickBot="1">
+    <row r="283" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A283" s="19">
         <v>7638</v>
       </c>
@@ -5339,7 +5368,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="18" thickBot="1">
+    <row r="284" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A284" s="19">
         <v>7639</v>
       </c>
@@ -5351,7 +5380,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="18" thickBot="1">
+    <row r="285" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A285" s="19">
         <v>7640</v>
       </c>
@@ -5363,7 +5392,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="18" thickBot="1">
+    <row r="286" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A286" s="19">
         <v>7641</v>
       </c>
@@ -5375,7 +5404,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="18" thickBot="1">
+    <row r="287" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A287" s="19">
         <v>7642</v>
       </c>
@@ -5387,7 +5416,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="18" thickBot="1">
+    <row r="288" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A288" s="19">
         <v>7643</v>
       </c>
@@ -5399,7 +5428,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="18" thickBot="1">
+    <row r="289" spans="1:4" ht="17" hidden="1" thickBot="1">
       <c r="A289" s="19">
         <v>7644</v>
       </c>
@@ -5411,7 +5440,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="18" thickBot="1">
+    <row r="290" spans="1:4" ht="18" hidden="1" thickBot="1">
       <c r="A290" s="30">
         <v>1949</v>
       </c>
@@ -5423,7 +5452,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:4" ht="18" thickBot="1">
       <c r="A291" s="30">
         <v>7433</v>
       </c>
@@ -5432,6 +5461,54 @@
       </c>
       <c r="C291" s="32"/>
       <c r="D291" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" ht="18" thickBot="1">
+      <c r="A292" s="30">
+        <v>7452</v>
+      </c>
+      <c r="B292" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C292" s="32"/>
+      <c r="D292" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" ht="18" thickBot="1">
+      <c r="A293" s="30">
+        <v>7296</v>
+      </c>
+      <c r="B293" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="C293" s="32"/>
+      <c r="D293" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" ht="18" thickBot="1">
+      <c r="A294" s="30">
+        <v>7298</v>
+      </c>
+      <c r="B294" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="C294" s="32"/>
+      <c r="D294" s="33">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" ht="17">
+      <c r="A295" s="1">
+        <v>6156</v>
+      </c>
+      <c r="B295" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C295" s="32"/>
+      <c r="D295" s="33">
         <v>226</v>
       </c>
     </row>

</xml_diff>